<commit_message>
Add dados do dashboard em CSV
</commit_message>
<xml_diff>
--- a/01_dashboard/data/AreaRuralVSUrbana.xlsx
+++ b/01_dashboard/data/AreaRuralVSUrbana.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bakerhughes-my.sharepoint.com/personal/gabriel_salgueiro2_bakerhughes_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielsalgueiro/Documents/meli_vagaAE/01_dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="8_{ED8EDB6E-24A1-4943-955D-3A8FB4CB63A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9ABCAD1A-37BA-4F66-9201-C505344059FE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EB1E9E-1145-984C-985B-672A16D8DD85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{4A29647E-15F8-43BF-8CB6-FE6971235462}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="25600" windowHeight="14780" xr2:uid="{4A29647E-15F8-43BF-8CB6-FE6971235462}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,6 +116,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -193,18 +194,18 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -264,7 +265,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -583,12 +584,12 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="71.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="58" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -619,10 +620,10 @@
       <c r="C2" s="2">
         <v>19248981</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="3">
         <v>19900257</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="1">
         <f>C2/D2</f>
         <v>0.96727298546948415</v>
       </c>
@@ -637,10 +638,10 @@
       <c r="C3" s="2">
         <v>19820773</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="3">
         <v>20083740</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="1">
         <f t="shared" ref="E3:E43" si="0">C3/D3</f>
         <v>0.98690647259922704</v>
       </c>
@@ -655,10 +656,10 @@
       <c r="C4" s="2">
         <v>20355918</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="3">
         <v>20264439</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1">
         <f t="shared" si="0"/>
         <v>1.0045142626450208</v>
       </c>
@@ -673,10 +674,10 @@
       <c r="C5" s="2">
         <v>19358702</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="3">
         <v>20442173</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <f t="shared" si="0"/>
         <v>0.94699824720199755</v>
       </c>
@@ -691,10 +692,10 @@
       <c r="C6" s="2">
         <v>20560976</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="3">
         <v>20616787</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <f t="shared" si="0"/>
         <v>0.9972929341511847</v>
       </c>
@@ -709,10 +710,10 @@
       <c r="C7" s="2">
         <v>21824888</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="3">
         <v>20788434</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <f t="shared" si="0"/>
         <v>1.0498572427341089</v>
       </c>
@@ -727,10 +728,10 @@
       <c r="C8" s="2">
         <v>23015233</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="3">
         <v>20957293</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <f t="shared" si="0"/>
         <v>1.0981968425025121</v>
       </c>
@@ -745,10 +746,10 @@
       <c r="C9" s="2">
         <v>3265460</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="3">
         <v>3645321</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="1">
         <f t="shared" si="0"/>
         <v>0.89579491079112095</v>
       </c>
@@ -763,10 +764,10 @@
       <c r="C10" s="2">
         <v>3441268</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="3">
         <v>3683937</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="1">
         <f t="shared" si="0"/>
         <v>0.93412780946036811</v>
       </c>
@@ -781,10 +782,10 @@
       <c r="C11" s="2">
         <v>3404680</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="3">
         <v>3722332</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="1">
         <f t="shared" si="0"/>
         <v>0.91466317351595716</v>
       </c>
@@ -799,10 +800,10 @@
       <c r="C12" s="2">
         <v>3320763</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="3">
         <v>3760450</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="1">
         <f t="shared" si="0"/>
         <v>0.88307596165352553</v>
       </c>
@@ -817,10 +818,10 @@
       <c r="C13" s="2">
         <v>3563597</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="3">
         <v>3798261</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="1">
         <f t="shared" si="0"/>
         <v>0.93821804241467344</v>
       </c>
@@ -835,10 +836,10 @@
       <c r="C14" s="2">
         <v>3777556</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="3">
         <v>3835738</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="1">
         <f t="shared" si="0"/>
         <v>0.98483160215843735</v>
       </c>
@@ -853,10 +854,10 @@
       <c r="C15" s="2">
         <v>3917474</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="3">
         <v>3872830</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="1">
         <f t="shared" si="0"/>
         <v>1.0115274876511491</v>
       </c>
@@ -871,10 +872,10 @@
       <c r="C16" s="2">
         <v>743305</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="3">
         <v>1168165</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="1">
         <f t="shared" si="0"/>
         <v>0.63630137865798064</v>
       </c>
@@ -889,10 +890,10 @@
       <c r="C17" s="2">
         <v>819993</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="3">
         <v>1180477</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="1">
         <f t="shared" si="0"/>
         <v>0.69462852728176827</v>
       </c>
@@ -907,10 +908,10 @@
       <c r="C18" s="2">
         <v>825120</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="3">
         <v>1192616</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="1">
         <f t="shared" si="0"/>
         <v>0.69185722814384509</v>
       </c>
@@ -925,10 +926,10 @@
       <c r="C19" s="2">
         <v>819772</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="3">
         <v>1204541</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="1">
         <f t="shared" si="0"/>
         <v>0.68056795077959154</v>
       </c>
@@ -943,10 +944,10 @@
       <c r="C20" s="2">
         <v>864688</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="3">
         <v>1216247</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="1">
         <f t="shared" si="0"/>
         <v>0.71094769401281155</v>
       </c>
@@ -961,10 +962,10 @@
       <c r="C21" s="2">
         <v>950730</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="3">
         <v>1227736</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="1">
         <f t="shared" si="0"/>
         <v>0.77437657607172883</v>
       </c>
@@ -979,10 +980,10 @@
       <c r="C22" s="2">
         <v>1005678</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="3">
         <v>1238989</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="1">
         <f t="shared" si="0"/>
         <v>0.81169243633317167</v>
       </c>
@@ -1000,7 +1001,7 @@
       <c r="D23" s="4">
         <v>948172</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="1">
         <f t="shared" si="0"/>
         <v>0.55449222293001688</v>
       </c>
@@ -1018,7 +1019,7 @@
       <c r="D24" s="4">
         <v>958251</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="1">
         <f t="shared" si="0"/>
         <v>0.59382249535873166</v>
       </c>
@@ -1036,7 +1037,7 @@
       <c r="D25" s="4">
         <v>968309</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="1">
         <f t="shared" si="0"/>
         <v>0.59524800451095672</v>
       </c>
@@ -1054,7 +1055,7 @@
       <c r="D26" s="4">
         <v>978313</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="1">
         <f t="shared" si="0"/>
         <v>0.59512957509508713</v>
       </c>
@@ -1072,7 +1073,7 @@
       <c r="D27" s="4">
         <v>988245</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="1">
         <f t="shared" si="0"/>
         <v>0.6346543620256111</v>
       </c>
@@ -1090,7 +1091,7 @@
       <c r="D28" s="4">
         <v>998093</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="1">
         <f t="shared" si="0"/>
         <v>0.70129937791368135</v>
       </c>
@@ -1108,7 +1109,7 @@
       <c r="D29" s="4">
         <v>1007830</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="1">
         <f t="shared" si="0"/>
         <v>0.7403778415010468</v>
       </c>
@@ -1126,7 +1127,7 @@
       <c r="D30" s="5">
         <v>3453674</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="1">
         <f t="shared" si="0"/>
         <v>0.82628383570655484</v>
       </c>
@@ -1144,7 +1145,7 @@
       <c r="D31" s="5">
         <v>3481514</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="1">
         <f t="shared" si="0"/>
         <v>0.85599914290162271</v>
       </c>
@@ -1162,7 +1163,7 @@
       <c r="D32" s="5">
         <v>3509113</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="1">
         <f t="shared" si="0"/>
         <v>0.85656916719410292</v>
       </c>
@@ -1180,7 +1181,7 @@
       <c r="D33" s="5">
         <v>3536418</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="1">
         <f t="shared" si="0"/>
         <v>0.83923817829227199</v>
       </c>
@@ -1198,7 +1199,7 @@
       <c r="D34" s="5">
         <v>3563390</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="1">
         <f t="shared" si="0"/>
         <v>0.87965055747476417</v>
       </c>
@@ -1216,7 +1217,7 @@
       <c r="D35" s="5">
         <v>3589999</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35" s="1">
         <f t="shared" si="0"/>
         <v>0.92733814131981651</v>
       </c>
@@ -1234,7 +1235,7 @@
       <c r="D36" s="5">
         <v>3616227</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="1">
         <f t="shared" si="0"/>
         <v>0.94025762210170982</v>
       </c>
@@ -1252,7 +1253,7 @@
       <c r="D37" s="6">
         <v>589916</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37" s="1">
         <f t="shared" si="0"/>
         <v>0.6036062761477905</v>
       </c>
@@ -1270,7 +1271,7 @@
       <c r="D38" s="6">
         <v>595129</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38" s="1">
         <f t="shared" si="0"/>
         <v>0.65180322249461886</v>
       </c>
@@ -1288,7 +1289,7 @@
       <c r="D39" s="6">
         <v>600229</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39" s="1">
         <f t="shared" si="0"/>
         <v>0.65310573131254901</v>
       </c>
@@ -1306,7 +1307,7 @@
       <c r="D40" s="6">
         <v>605193</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="1">
         <f t="shared" si="0"/>
         <v>0.63671919536412347</v>
       </c>
@@ -1324,7 +1325,7 @@
       <c r="D41" s="6">
         <v>610019</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="1">
         <f t="shared" si="0"/>
         <v>0.66786280427330957</v>
       </c>
@@ -1342,7 +1343,7 @@
       <c r="D42" s="6">
         <v>614706</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="1">
         <f t="shared" si="0"/>
         <v>0.73372311316304051</v>
       </c>
@@ -1360,7 +1361,7 @@
       <c r="D43" s="6">
         <v>619240</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="1">
         <f t="shared" si="0"/>
         <v>0.78422905497060913</v>
       </c>

</xml_diff>